<commit_message>
Added more web service methods
</commit_message>
<xml_diff>
--- a/Movies/Docs/CodeGen.xlsx
+++ b/Movies/Docs/CodeGen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Chaosg5\Chaos\Movies\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B794FAC-7E1A-4375-A74B-1ACF2466F86E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A55CA3-F9D8-493E-ADB1-447CBE5C6720}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="4425" xr2:uid="{A9CB4FE8-BCC1-4058-B451-CC71A7F527DA}"/>
   </bookViews>
@@ -204,9 +204,6 @@
     <t>Typeable</t>
   </si>
   <si>
-    <t>Persistable</t>
-  </si>
-  <si>
     <t>Collectable</t>
   </si>
   <si>
@@ -343,6 +340,9 @@
   </si>
   <si>
     <t>Variable name</t>
+  </si>
+  <si>
+    <t>Persitable</t>
   </si>
 </sst>
 </file>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDB9D36-31E7-41C6-A118-35151D6ECB7D}">
   <dimension ref="A1:AG176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4:AG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>42</v>
@@ -894,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>57</v>
@@ -1025,7 +1025,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>58</v>
@@ -1156,26 +1156,26 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="D4" s="5" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>#region Error</v>
       </c>
       <c r="E4" s="6" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v xml:space="preserve">/// &lt;inheritdoc /&gt; /// &lt;exception cref="FaultException"&gt;An exception occurred.&lt;/exception&gt; public async Task ErrorSaveAsync(UserSessionDto session, ErrorDto error) { try { </v>
       </c>
       <c r="F4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>this.ValidateStateAndSession(session); await Error.Static.FromContract(error).SaveAsync(UserSession.Static.FromContract(session)); } catch (Exception exception) { throw new FaultException</v>
       </c>
       <c r="G4" s="6" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>(exception.Message); } }</v>
       </c>
       <c r="H4" s="6" t="str">
         <f t="shared" si="4"/>
@@ -1223,19 +1223,19 @@
       </c>
       <c r="S4" s="7" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>#endregion</v>
       </c>
       <c r="T4" s="5" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>#region Error</v>
       </c>
       <c r="U4" s="6" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>/// &lt;summary&gt;Saves the &lt;paramref name="error"/&gt;.&lt;/summary&gt; /// &lt;param name="session"&gt;The session.&lt;/param&gt; /// &lt;param name="error"&gt;The &lt;see cref="ErrorDto"/&gt; to save.&lt;/param&gt;</v>
       </c>
       <c r="V4" s="6" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>/// &lt;returns&gt;The &lt;see cref="Task"/&gt;.&lt;/returns&gt; [OperationContract] Task ErrorSaveAsync(UserSessionDto session, ErrorDto error);</v>
       </c>
       <c r="W4" s="6" t="str">
         <f t="shared" si="17"/>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="AG4" s="7" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>#endregion</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
@@ -1287,10 +1287,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1418,10 +1418,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1549,10 +1549,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1680,10 +1680,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1811,7 +1811,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
         <v>57</v>
@@ -1942,7 +1942,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
         <v>58</v>
@@ -2073,10 +2073,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2204,7 +2204,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
         <v>57</v>
@@ -2335,10 +2335,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2466,7 +2466,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
         <v>58</v>
@@ -2597,10 +2597,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2728,10 +2728,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2859,10 +2859,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2990,10 +2990,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="5" t="str">
         <f t="shared" si="0"/>
@@ -3121,7 +3121,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
         <v>57</v>
@@ -3252,10 +3252,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" s="5" t="str">
         <f t="shared" si="0"/>
@@ -3383,7 +3383,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s">
         <v>57</v>
@@ -3514,7 +3514,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
         <v>58</v>
@@ -3645,7 +3645,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
         <v>58</v>
@@ -3776,7 +3776,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
         <v>57</v>
@@ -3907,10 +3907,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" s="5" t="str">
         <f t="shared" si="0"/>
@@ -4038,10 +4038,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D26" s="5" t="str">
         <f t="shared" si="0"/>
@@ -4169,10 +4169,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" s="5" t="str">
         <f t="shared" si="0"/>
@@ -4300,10 +4300,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28" s="5" t="str">
         <f t="shared" si="0"/>
@@ -4431,7 +4431,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" t="s">
         <v>58</v>
@@ -4562,7 +4562,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
         <v>58</v>
@@ -4693,10 +4693,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D31" s="5" t="str">
         <f t="shared" si="0"/>
@@ -4824,10 +4824,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D32" s="5" t="str">
         <f t="shared" si="0"/>
@@ -4955,7 +4955,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C33" t="s">
         <v>58</v>
@@ -5086,10 +5086,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" s="5" t="str">
         <f t="shared" si="0"/>
@@ -5217,7 +5217,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C35" t="s">
         <v>57</v>
@@ -5348,10 +5348,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D36" s="5" t="str">
         <f t="shared" si="0"/>
@@ -5479,10 +5479,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D37" s="5" t="str">
         <f t="shared" si="0"/>
@@ -5610,26 +5610,26 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C38" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="D38" s="5" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>#region UserSession</v>
       </c>
       <c r="E38" s="6" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v xml:space="preserve">/// &lt;inheritdoc /&gt; /// &lt;exception cref="FaultException"&gt;An exception occurred.&lt;/exception&gt; public async Task UserSessionSaveAsync(UserSessionDto session, UserSessionDto userSession) { try { </v>
       </c>
       <c r="F38" s="6" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>this.ValidateStateAndSession(session); await UserSession.Static.FromContract(userSession).SaveAsync(UserSession.Static.FromContract(session)); } catch (Exception exception) { throw new FaultException</v>
       </c>
       <c r="G38" s="6" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>(exception.Message); } }</v>
       </c>
       <c r="H38" s="6" t="str">
         <f t="shared" si="4"/>
@@ -5677,19 +5677,19 @@
       </c>
       <c r="S38" s="7" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>#endregion</v>
       </c>
       <c r="T38" s="5" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>#region UserSession</v>
       </c>
       <c r="U38" s="6" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>/// &lt;summary&gt;Saves the &lt;paramref name="userSession"/&gt;.&lt;/summary&gt; /// &lt;param name="session"&gt;The session.&lt;/param&gt; /// &lt;param name="userSession"&gt;The &lt;see cref="UserSessionDto"/&gt; to save.&lt;/param&gt;</v>
       </c>
       <c r="V38" s="6" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>/// &lt;returns&gt;The &lt;see cref="Task"/&gt;.&lt;/returns&gt; [OperationContract] Task UserSessionSaveAsync(UserSessionDto session, UserSessionDto userSession);</v>
       </c>
       <c r="W38" s="6" t="str">
         <f t="shared" si="17"/>
@@ -5733,7 +5733,7 @@
       </c>
       <c r="AG38" s="7" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>#endregion</v>
       </c>
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.25">
@@ -5741,10 +5741,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D39" s="5" t="str">
         <f t="shared" si="0"/>
@@ -5872,7 +5872,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C40" t="s">
         <v>57</v>
@@ -6003,7 +6003,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C41" t="s">
         <v>58</v>
@@ -6134,7 +6134,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C42" t="s">
         <v>58</v>
@@ -10166,51 +10166,51 @@
     </row>
     <row r="75" spans="4:33" x14ac:dyDescent="0.25">
       <c r="D75" s="5" t="str">
-        <f t="shared" ref="D67:D130" si="52">IF(COUNTIF(E75:R75,"")&lt;13,"#region","")</f>
+        <f t="shared" ref="D75:D130" si="52">IF(COUNTIF(E75:R75,"")&lt;13,"#region","")</f>
         <v/>
       </c>
       <c r="E75" s="6" t="str">
-        <f t="shared" ref="E67:E130" si="53">IF(OR(C75="Typeable",C75="Readable",C75="Persitable"),"/// &lt;inheritdoc /&gt; /// &lt;exception cref=""FaultException""&gt;An exception occurred.&lt;/exception&gt; public async Task "&amp;A75&amp;"SaveAsync(UserSessionDto session, "&amp;A75&amp;"Dto "&amp;B75&amp;") { try { ","")</f>
+        <f t="shared" ref="E75:E130" si="53">IF(OR(C75="Typeable",C75="Readable",C75="Persitable"),"/// &lt;inheritdoc /&gt; /// &lt;exception cref=""FaultException""&gt;An exception occurred.&lt;/exception&gt; public async Task "&amp;A75&amp;"SaveAsync(UserSessionDto session, "&amp;A75&amp;"Dto "&amp;B75&amp;") { try { ","")</f>
         <v/>
       </c>
       <c r="F75" s="6" t="str">
-        <f t="shared" ref="F67:F130" si="54">IF(OR(C75="Typeable",C75="Readable",C75="Persitable"),"this.ValidateStateAndSession(session); await "&amp;A75&amp;".Static.FromContract("&amp;B75&amp;").SaveAsync(UserSession.Static.FromContract(session)); } catch (Exception exception) { throw new FaultException","")</f>
+        <f t="shared" ref="F75:F130" si="54">IF(OR(C75="Typeable",C75="Readable",C75="Persitable"),"this.ValidateStateAndSession(session); await "&amp;A75&amp;".Static.FromContract("&amp;B75&amp;").SaveAsync(UserSession.Static.FromContract(session)); } catch (Exception exception) { throw new FaultException","")</f>
         <v/>
       </c>
       <c r="H75" s="6" t="str">
-        <f t="shared" ref="H67:H130" si="55">IF(OR(C75="Storeable"),"(exception.Message); } } /// &lt;inheritdoc /&gt; /// &lt;exception cref=""FaultException""&gt;An exception occurred.&lt;/exception&gt; public async Task "&amp;A75&amp;"SaveAllAsync(UserSessionDto session, "&amp;A75&amp;"Dto "&amp;B75&amp;") { try ","")</f>
+        <f t="shared" ref="H75:H130" si="55">IF(OR(C75="Storeable"),"(exception.Message); } } /// &lt;inheritdoc /&gt; /// &lt;exception cref=""FaultException""&gt;An exception occurred.&lt;/exception&gt; public async Task "&amp;A75&amp;"SaveAllAsync(UserSessionDto session, "&amp;A75&amp;"Dto "&amp;B75&amp;") { try ","")</f>
         <v/>
       </c>
       <c r="I75" s="6" t="str">
-        <f t="shared" ref="I67:I130" si="56">IF(OR(C75="Storeable"),"{ this.ValidateStateAndSession(session); await "&amp;A75&amp;".Static.SaveAllAsync(UserSession.Static.FromContract(session)); } catch (Exception exception) { throw new FaultException(exception.Message); } }","")</f>
+        <f t="shared" ref="I75:I130" si="56">IF(OR(C75="Storeable"),"{ this.ValidateStateAndSession(session); await "&amp;A75&amp;".Static.SaveAllAsync(UserSession.Static.FromContract(session)); } catch (Exception exception) { throw new FaultException(exception.Message); } }","")</f>
         <v/>
       </c>
       <c r="J75" s="6" t="str">
-        <f t="shared" ref="J67:J130" si="57">IF(OR(C75="Typeable",C75="Readable"),"/// &lt;inheritdoc /&gt; /// &lt;exception cref=""FaultException""&gt;An exception occurred.&lt;/exception&gt; public async Task&lt;IEnumerable&lt;"&amp;A75&amp;"Dto&gt;&gt; "&amp;A75&amp;"GetAsync(UserSessionDto session, ","")</f>
+        <f t="shared" ref="J75:J130" si="57">IF(OR(C75="Typeable",C75="Readable"),"/// &lt;inheritdoc /&gt; /// &lt;exception cref=""FaultException""&gt;An exception occurred.&lt;/exception&gt; public async Task&lt;IEnumerable&lt;"&amp;A75&amp;"Dto&gt;&gt; "&amp;A75&amp;"GetAsync(UserSessionDto session, ","")</f>
         <v/>
       </c>
       <c r="K75" s="6" t="str">
-        <f t="shared" ref="K67:K130" si="58">IF(OR(C75="Typeable",C75="Readable"),"IEnumerable&lt;int&gt; idList) { try { this.ValidateStateAndSession(session); return (await "&amp;A75&amp;".Static.GetAsync(UserSession.Static.FromContract(session), idList)).Select(c =&gt; c.ToContract()); }","")</f>
+        <f t="shared" ref="K75:K130" si="58">IF(OR(C75="Typeable",C75="Readable"),"IEnumerable&lt;int&gt; idList) { try { this.ValidateStateAndSession(session); return (await "&amp;A75&amp;".Static.GetAsync(UserSession.Static.FromContract(session), idList)).Select(c =&gt; c.ToContract()); }","")</f>
         <v/>
       </c>
       <c r="L75" s="6" t="str">
-        <f t="shared" ref="L67:L130" si="59">IF(OR(C75="Typeable",C75="Readable"),"catch (Exception exception) { throw new FaultException(exception.Message); } }","")</f>
+        <f t="shared" ref="L75:L130" si="59">IF(OR(C75="Typeable",C75="Readable"),"catch (Exception exception) { throw new FaultException(exception.Message); } }","")</f>
         <v/>
       </c>
       <c r="M75" s="6" t="str">
-        <f t="shared" ref="M67:M130" si="60">IF(OR(C75="Typeable"),"/// &lt;inheritdoc /&gt; /// &lt;exception cref=""FaultException""&gt;An exception occurred.&lt;/exception&gt; public async Task&lt;IEnumerable&lt;"&amp;A75&amp;"Dto&gt;&gt; "&amp;A75&amp;"GetAllAsync(UserSessionDto session) { try { this.ValidateStateAndSession(session); ","")</f>
+        <f t="shared" ref="M75:M130" si="60">IF(OR(C75="Typeable"),"/// &lt;inheritdoc /&gt; /// &lt;exception cref=""FaultException""&gt;An exception occurred.&lt;/exception&gt; public async Task&lt;IEnumerable&lt;"&amp;A75&amp;"Dto&gt;&gt; "&amp;A75&amp;"GetAllAsync(UserSessionDto session) { try { this.ValidateStateAndSession(session); ","")</f>
         <v/>
       </c>
       <c r="N75" s="6" t="str">
-        <f t="shared" ref="N67:N130" si="61">IF(OR(C75="Typeable"),"return (await "&amp;A75&amp;".Static.GetAllAsync(UserSession.Static.FromContract(session))).Select(c =&gt; c.ToContract()); } catch (Exception exception) { throw new FaultException(exception.Message); } }","")</f>
+        <f t="shared" ref="N75:N130" si="61">IF(OR(C75="Typeable"),"return (await "&amp;A75&amp;".Static.GetAllAsync(UserSession.Static.FromContract(session))).Select(c =&gt; c.ToContract()); } catch (Exception exception) { throw new FaultException(exception.Message); } }","")</f>
         <v/>
       </c>
       <c r="O75" s="6" t="str">
-        <f t="shared" ref="O67:O130" si="62">IF(OR(C75="Collectable"),"/// &lt;inheritdoc /&gt; /// &lt;exception cref=""FaultException""&gt;An exception occurred.&lt;/exception&gt; public async Task "&amp;A75&amp;"SaveAsync(UserSessionDto session, "&amp;A75&amp;"Dto "&amp;B75&amp;") { try { ","")</f>
+        <f t="shared" ref="O75:O130" si="62">IF(OR(C75="Collectable"),"/// &lt;inheritdoc /&gt; /// &lt;exception cref=""FaultException""&gt;An exception occurred.&lt;/exception&gt; public async Task "&amp;A75&amp;"SaveAsync(UserSessionDto session, "&amp;A75&amp;"Dto "&amp;B75&amp;") { try { ","")</f>
         <v/>
       </c>
       <c r="P75" s="6" t="str">
-        <f t="shared" ref="P67:P130" si="63">IF(OR(C75="Collectable"),"this.ValidateStateAndSession(session); await "&amp;A75&amp;".Static.FromContract("&amp;B75&amp;").SaveAsync(UserSession.Static.FromContract(session)); } catch (Exception exception) { throw new FaultException","")</f>
+        <f t="shared" ref="P75:P130" si="63">IF(OR(C75="Collectable"),"this.ValidateStateAndSession(session); await "&amp;A75&amp;".Static.FromContract("&amp;B75&amp;").SaveAsync(UserSession.Static.FromContract(session)); } catch (Exception exception) { throw new FaultException","")</f>
         <v/>
       </c>
       <c r="Q75" s="6" t="str">
@@ -10222,51 +10222,51 @@
         <v/>
       </c>
       <c r="S75" s="7" t="str">
-        <f t="shared" ref="S67:S130" si="64">IF(COUNTIF(E75:R75,"")&lt;13,"#endregion","")</f>
+        <f t="shared" ref="S75:S130" si="64">IF(COUNTIF(E75:R75,"")&lt;13,"#endregion","")</f>
         <v/>
       </c>
       <c r="T75" s="5" t="str">
-        <f t="shared" ref="T67:T130" si="65">IF(COUNTIF(U75:AF75,"")&lt;12,"#region","")</f>
+        <f t="shared" ref="T75:T130" si="65">IF(COUNTIF(U75:AF75,"")&lt;12,"#region","")</f>
         <v/>
       </c>
       <c r="U75" s="6" t="str">
-        <f t="shared" ref="U67:U130" si="66">IF(OR(C75="Typeable",C75="Readable",C75="Persitable"),"/// &lt;summary&gt;Saves the &lt;paramref name="""&amp;B75&amp;"""/&gt;.&lt;/summary&gt; /// &lt;param name=""session""&gt;The session.&lt;/param&gt; /// &lt;param name="""&amp;B75&amp;"""&gt;The &lt;see cref="""&amp;A75&amp;"Dto""/&gt; to save.&lt;/param&gt;","")</f>
+        <f t="shared" ref="U75:U130" si="66">IF(OR(C75="Typeable",C75="Readable",C75="Persitable"),"/// &lt;summary&gt;Saves the &lt;paramref name="""&amp;B75&amp;"""/&gt;.&lt;/summary&gt; /// &lt;param name=""session""&gt;The session.&lt;/param&gt; /// &lt;param name="""&amp;B75&amp;"""&gt;The &lt;see cref="""&amp;A75&amp;"Dto""/&gt; to save.&lt;/param&gt;","")</f>
         <v/>
       </c>
       <c r="V75" s="6" t="str">
-        <f t="shared" ref="V67:V130" si="67">IF(OR(C75="Typeable",C75="Readable",C75="Persitable"),"/// &lt;returns&gt;The &lt;see cref=""Task""/&gt;.&lt;/returns&gt; [OperationContract] Task "&amp;A75&amp;"SaveAsync(UserSessionDto session, "&amp;A75&amp;"Dto "&amp;B75&amp;");","")</f>
+        <f t="shared" ref="V75:V130" si="67">IF(OR(C75="Typeable",C75="Readable",C75="Persitable"),"/// &lt;returns&gt;The &lt;see cref=""Task""/&gt;.&lt;/returns&gt; [OperationContract] Task "&amp;A75&amp;"SaveAsync(UserSessionDto session, "&amp;A75&amp;"Dto "&amp;B75&amp;");","")</f>
         <v/>
       </c>
       <c r="W75" s="6" t="str">
-        <f t="shared" ref="W67:W130" si="68">IF(OR(C75="Storeable"),"/// &lt;summary&gt;Saves the &lt;paramref name="""&amp;B75&amp;"""/&gt; and all it's children.&lt;/summary&gt; /// &lt;param name=""session""&gt;The session.&lt;/param&gt;","")</f>
+        <f t="shared" ref="W75:W130" si="68">IF(OR(C75="Storeable"),"/// &lt;summary&gt;Saves the &lt;paramref name="""&amp;B75&amp;"""/&gt; and all it's children.&lt;/summary&gt; /// &lt;param name=""session""&gt;The session.&lt;/param&gt;","")</f>
         <v/>
       </c>
       <c r="X75" s="6" t="str">
-        <f t="shared" ref="X67:X130" si="69">IF(OR(C75="Storeable"),"/// &lt;param name="""&amp;B75&amp;"""&gt;The &lt;see cref="""&amp;A75&amp;"Dto""/&gt; to save.&lt;/param&gt; /// &lt;returns&gt;The &lt;see cref=""Task""/&gt;.&lt;/returns&gt; [OperationContract] Task "&amp;A75&amp;"SaveAllAsync(UserSessionDto session, "&amp;A75&amp;"Dto "&amp;B75&amp;");","")</f>
+        <f t="shared" ref="X75:X130" si="69">IF(OR(C75="Storeable"),"/// &lt;param name="""&amp;B75&amp;"""&gt;The &lt;see cref="""&amp;A75&amp;"Dto""/&gt; to save.&lt;/param&gt; /// &lt;returns&gt;The &lt;see cref=""Task""/&gt;.&lt;/returns&gt; [OperationContract] Task "&amp;A75&amp;"SaveAllAsync(UserSessionDto session, "&amp;A75&amp;"Dto "&amp;B75&amp;");","")</f>
         <v/>
       </c>
       <c r="Y75" s="6" t="str">
-        <f t="shared" ref="Y67:Y130" si="70">IF(OR(C75="Typeable",C75="Readable"),"/// &lt;summary&gt;Gets the &lt;see cref="""&amp;A75&amp;"Dto""/&gt; with the specified &lt;paramref name=""idList""/&gt;.&lt;/summary&gt; /// &lt;param name=""session""&gt;The session.&lt;/param&gt;/// &lt;param name=""idList""&gt;The id list.&lt;/param&gt;","")</f>
+        <f t="shared" ref="Y75:Y130" si="70">IF(OR(C75="Typeable",C75="Readable"),"/// &lt;summary&gt;Gets the &lt;see cref="""&amp;A75&amp;"Dto""/&gt; with the specified &lt;paramref name=""idList""/&gt;.&lt;/summary&gt; /// &lt;param name=""session""&gt;The session.&lt;/param&gt;/// &lt;param name=""idList""&gt;The id list.&lt;/param&gt;","")</f>
         <v/>
       </c>
       <c r="Z75" s="6" t="str">
-        <f t="shared" ref="Z67:Z130" si="71">IF(OR(C75="Typeable",C75="Readable"),"/// &lt;returns&gt;The &lt;see cref=""Task""/&gt;.&lt;/returns&gt; [OperationContract] Task&lt;IEnumerable&lt;"&amp;A75&amp;"Dto&gt;&gt; "&amp;A75&amp;"GetAsync(UserSessionDto session, IEnumerable&lt;int&gt; idList);","")</f>
+        <f t="shared" ref="Z75:Z130" si="71">IF(OR(C75="Typeable",C75="Readable"),"/// &lt;returns&gt;The &lt;see cref=""Task""/&gt;.&lt;/returns&gt; [OperationContract] Task&lt;IEnumerable&lt;"&amp;A75&amp;"Dto&gt;&gt; "&amp;A75&amp;"GetAsync(UserSessionDto session, IEnumerable&lt;int&gt; idList);","")</f>
         <v/>
       </c>
       <c r="AA75" s="6" t="str">
-        <f t="shared" ref="AA67:AA130" si="72">IF(OR(C75="Typeable"),"/// &lt;summary&gt;Gets all &lt;see cref="""&amp;A75&amp;"Dto""/&gt;s.&lt;/summary&gt; /// &lt;param name=""session""&gt;The session.&lt;/param&gt;","")</f>
+        <f t="shared" ref="AA75:AA130" si="72">IF(OR(C75="Typeable"),"/// &lt;summary&gt;Gets all &lt;see cref="""&amp;A75&amp;"Dto""/&gt;s.&lt;/summary&gt; /// &lt;param name=""session""&gt;The session.&lt;/param&gt;","")</f>
         <v/>
       </c>
       <c r="AB75" s="6" t="str">
-        <f t="shared" ref="AB67:AB130" si="73">IF(OR(C75="Typeable"),"/// &lt;returns&gt;The &lt;see cref=""Task""/&gt;.&lt;/returns&gt; [OperationContract] Task&lt;IEnumerable&lt;"&amp;A75&amp;"Dto&gt;&gt; "&amp;A75&amp;"GetAllAsync(UserSessionDto session);","")</f>
+        <f t="shared" ref="AB75:AB130" si="73">IF(OR(C75="Typeable"),"/// &lt;returns&gt;The &lt;see cref=""Task""/&gt;.&lt;/returns&gt; [OperationContract] Task&lt;IEnumerable&lt;"&amp;A75&amp;"Dto&gt;&gt; "&amp;A75&amp;"GetAllAsync(UserSessionDto session);","")</f>
         <v/>
       </c>
       <c r="AC75" s="6" t="str">
-        <f t="shared" ref="AC67:AC130" si="74">IF(OR(C75="Collectable"),"/// &lt;summary&gt;Saves the &lt;paramref name="""&amp;B75&amp;"""/&gt;.&lt;/summary&gt; /// &lt;param name=""session""&gt;The session.&lt;/param&gt; /// &lt;param name="""&amp;B75&amp;"""&gt;The &lt;see cref="""&amp;A75&amp;"Dto""/&gt; to save.&lt;/param&gt;","")</f>
+        <f t="shared" ref="AC75:AC130" si="74">IF(OR(C75="Collectable"),"/// &lt;summary&gt;Saves the &lt;paramref name="""&amp;B75&amp;"""/&gt;.&lt;/summary&gt; /// &lt;param name=""session""&gt;The session.&lt;/param&gt; /// &lt;param name="""&amp;B75&amp;"""&gt;The &lt;see cref="""&amp;A75&amp;"Dto""/&gt; to save.&lt;/param&gt;","")</f>
         <v/>
       </c>
       <c r="AD75" s="6" t="str">
-        <f t="shared" ref="AD67:AD130" si="75">IF(OR(C75="Collectable"),"/// &lt;returns&gt;The &lt;see cref=""Task""/&gt;.&lt;/returns&gt; [OperationContract] Task "&amp;A75&amp;"SaveAsync(UserSessionDto session, "&amp;A75&amp;"Dto "&amp;B75&amp;");","")</f>
+        <f t="shared" ref="AD75:AD130" si="75">IF(OR(C75="Collectable"),"/// &lt;returns&gt;The &lt;see cref=""Task""/&gt;.&lt;/returns&gt; [OperationContract] Task "&amp;A75&amp;"SaveAsync(UserSessionDto session, "&amp;A75&amp;"Dto "&amp;B75&amp;");","")</f>
         <v/>
       </c>
       <c r="AE75" s="6" t="str">
@@ -10278,7 +10278,7 @@
         <v/>
       </c>
       <c r="AG75" s="7" t="str">
-        <f t="shared" ref="AG67:AG130" si="76">IF(COUNTIF(U75:AF75,"")&lt;12,"#endregion","")</f>
+        <f t="shared" ref="AG75:AG130" si="76">IF(COUNTIF(U75:AF75,"")&lt;12,"#endregion","")</f>
         <v/>
       </c>
     </row>

</xml_diff>